<commit_message>
Removing 'star' for wildcard
The plan is to have a star indicate wildcards, and a fullword to
indicate anything, but for now, we'll assume it's all the start of words
</commit_message>
<xml_diff>
--- a/Data/Categories.xlsx
+++ b/Data/Categories.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\Categories\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projects\SentenceToCategories\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,9 +32,6 @@
     <t>List B</t>
   </si>
   <si>
-    <t>Happy</t>
-  </si>
-  <si>
     <t>Dog</t>
   </si>
   <si>
@@ -44,13 +41,16 @@
     <t>Cat</t>
   </si>
   <si>
-    <t>Funny</t>
-  </si>
-  <si>
     <t>Human</t>
   </si>
   <si>
-    <t>Intellingent</t>
+    <t>Hap</t>
+  </si>
+  <si>
+    <t>Funn</t>
+  </si>
+  <si>
+    <t>Intelli</t>
   </si>
 </sst>
 </file>
@@ -371,7 +371,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -389,26 +389,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>